<commit_message>
add new functions to libft and new tests
</commit_message>
<xml_diff>
--- a/libft/doc/Libft_Status_Features.xlsx
+++ b/libft/doc/Libft_Status_Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pmicloud-my.sharepoint.com/personal/ybensegh_pmintl_net/Documents/Documents/Perso/ybensegh42/libft/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{0DA03AC8-1340-411D-8535-28C753531D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1083DA1F-2666-45EA-94F4-82FA9687A8FB}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{2A1DAAD1-4C48-4832-A05C-C1D5FBA16C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA4BE5D7-66F8-4155-A7E7-E8EC4C654A66}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2825E143-7484-4902-A5DA-2E02CC4607B9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="44">
   <si>
     <t>• bzero</t>
   </si>
@@ -142,13 +142,40 @@
   </si>
   <si>
     <t>Not Pass</t>
+  </si>
+  <si>
+    <t>Percentage of completion</t>
+  </si>
+  <si>
+    <t>First part</t>
+  </si>
+  <si>
+    <t>Half</t>
+  </si>
+  <si>
+    <t>Need to be validated versus strlcpy</t>
+  </si>
+  <si>
+    <t>Need to be validated versus strlcat</t>
+  </si>
+  <si>
+    <t>Need to be validated versus strnstr</t>
+  </si>
+  <si>
+    <t>Done Flag</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +187,13 @@
       <b/>
       <i/>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -199,18 +233,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -233,11 +273,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3A3E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -283,46 +343,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -341,28 +361,13 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC3A3E1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -671,383 +676,569 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6849B1-9256-4202-9C9C-A31FC936F1C6}">
-  <dimension ref="B2:F27"/>
+  <dimension ref="B2:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.26953125" customWidth="1"/>
+    <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C5" s="2" t="s">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C6" s="1" t="s">
+      <c r="H7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C7" s="1" t="s">
+      <c r="F8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="F9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C9" s="1" t="s">
+      <c r="F10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C10" s="1" t="s">
+      <c r="F11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C11" s="1" t="s">
+      <c r="F12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C12" s="1" t="s">
+      <c r="F13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C13" s="1" t="s">
+      <c r="F14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="E15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G15" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C14" s="1" t="s">
+      <c r="H15" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="E16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G16" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C15" s="1" t="s">
+      <c r="H16" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C23" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>34</v>
+      <c r="F29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <f>SUM(B7:B29)</f>
+        <v>23</v>
+      </c>
+      <c r="H30">
+        <f>SUM(H7:H29)</f>
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="I32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I33" s="3">
+        <f>H30/B30</f>
+        <v>0.42391304347826086</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Not Done">
-      <formula>NOT(ISERROR(SEARCH("Not Done",D1)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Not Done">
+      <formula>NOT(ISERROR(SEARCH("Not Done",E1)))</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:F27">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+  <conditionalFormatting sqref="E8:G29">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"na"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Half">
+      <formula>NOT(ISERROR(SEARCH("Half",F1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Valid"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Not pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update code and add new functions
</commit_message>
<xml_diff>
--- a/libft/doc/Libft_Status_Features.xlsx
+++ b/libft/doc/Libft_Status_Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pmicloud-my.sharepoint.com/personal/ybensegh_pmintl_net/Documents/Documents/Perso/ybensegh42/libft/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{2A1DAAD1-4C48-4832-A05C-C1D5FBA16C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA4BE5D7-66F8-4155-A7E7-E8EC4C654A66}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="13_ncr:1_{2A1DAAD1-4C48-4832-A05C-C1D5FBA16C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F0F788E-7091-453E-A145-DADB61CA758B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2825E143-7484-4902-A5DA-2E02CC4607B9}"/>
   </bookViews>
@@ -114,9 +114,6 @@
     <t>Last Update</t>
   </si>
   <si>
-    <t>10.04.2022</t>
-  </si>
-  <si>
     <t>Norminette</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>10.05.2022</t>
   </si>
 </sst>
 </file>
@@ -173,7 +173,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -241,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -250,7 +250,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC3A3E1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -318,16 +348,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -678,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6849B1-9256-4202-9C9C-A31FC936F1C6}">
   <dimension ref="B2:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -688,10 +708,10 @@
     <col min="3" max="3" width="10.6328125" customWidth="1"/>
     <col min="4" max="4" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.26953125" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.35">
@@ -707,12 +727,12 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">
@@ -723,19 +743,19 @@
         <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
@@ -746,15 +766,17 @@
         <v>21</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.75</v>
+      </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
@@ -765,15 +787,17 @@
         <v>0</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.75</v>
+      </c>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.35">
@@ -784,15 +808,17 @@
         <v>1</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.75</v>
+      </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.35">
@@ -803,15 +829,17 @@
         <v>2</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.75</v>
+      </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.35">
@@ -822,15 +850,17 @@
         <v>3</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.75</v>
+      </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
@@ -841,15 +871,17 @@
         <v>4</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0.75</v>
+      </c>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
@@ -860,13 +892,13 @@
         <v>5</v>
       </c>
       <c r="E14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -879,13 +911,13 @@
         <v>6</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="4">
         <v>0.75</v>
@@ -900,13 +932,13 @@
         <v>7</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H16" s="4">
         <v>0.75</v>
@@ -921,13 +953,13 @@
         <v>8</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H17" s="4">
         <v>0.75</v>
@@ -942,13 +974,13 @@
         <v>9</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H18" s="4">
         <v>0.75</v>
@@ -963,13 +995,13 @@
         <v>10</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H19" s="4">
         <v>0.75</v>
@@ -984,13 +1016,13 @@
         <v>11</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H20" s="4">
         <v>0.75</v>
@@ -1005,13 +1037,13 @@
         <v>12</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H21" s="4">
         <v>0.75</v>
@@ -1026,13 +1058,13 @@
         <v>13</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H22" s="4">
         <v>0.75</v>
@@ -1047,13 +1079,13 @@
         <v>14</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H23" s="4">
         <v>0.75</v>
@@ -1068,13 +1100,13 @@
         <v>15</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H24" s="4">
         <v>0.75</v>
@@ -1089,13 +1121,13 @@
         <v>16</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H25" s="4">
         <v>0.75</v>
@@ -1110,19 +1142,19 @@
         <v>17</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H26" s="4">
         <v>0.5</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.35">
@@ -1133,19 +1165,19 @@
         <v>18</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H27" s="4">
         <v>0.5</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.35">
@@ -1156,19 +1188,19 @@
         <v>19</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H28" s="4">
         <v>0.5</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.35">
@@ -1179,15 +1211,17 @@
         <v>20</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0.75</v>
+      </c>
       <c r="I29" s="4"/>
     </row>
     <row r="30" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
@@ -1197,44 +1231,47 @@
       </c>
       <c r="H30">
         <f>SUM(H7:H29)</f>
-        <v>9.75</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I33" s="3">
         <f>H30/B30</f>
-        <v>0.42391304347826086</v>
+        <v>0.65217391304347827</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Not Done">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Not Done">
       <formula>NOT(ISERROR(SEARCH("Not Done",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:G29">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
       <formula>"na"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Half">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Half">
       <formula>NOT(ISERROR(SEARCH("Half",F1)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Valid"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Not valid"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"Not pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add substr and start part two
</commit_message>
<xml_diff>
--- a/libft/doc/Libft_Status_Features.xlsx
+++ b/libft/doc/Libft_Status_Features.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="58">
   <si>
     <t xml:space="preserve">Author</t>
   </si>
@@ -155,6 +155,45 @@
   </si>
   <si>
     <t xml:space="preserve">• strdup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second Part</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ft_substr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ft_strjoin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ft_strtrim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ft_split</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ft_itoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ft_strmapi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ft_putchar_fd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ft_putstr_fd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ft_putendl_fd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ft_putnbr_fd</t>
   </si>
 </sst>
 </file>
@@ -423,8 +462,8 @@
   </sheetPr>
   <dimension ref="B2:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H56" activeCellId="0" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1028,6 +1067,279 @@
       </c>
       <c r="I37" s="3"/>
     </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D42" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H50" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H51" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H53" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="0" t="n">
+        <f aca="false">SUM(B44:B54)</f>
+        <v>11</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <f aca="false">SUM(H45:H54)</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I57" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I58" s="4" t="n">
+        <f aca="false">H55/B55</f>
+        <v>0.0681818181818182</v>
+      </c>
+    </row>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1057,7 +1369,7 @@
       <formula>NOT(ISERROR(SEARCH("Not Done",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:G29 E36:G37">
+  <conditionalFormatting sqref="E8:G29 E36:G37 E45:G54">
     <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"na"</formula>
     </cfRule>

</xml_diff>

<commit_message>
add new functions and fix toupper
</commit_message>
<xml_diff>
--- a/libft/doc/Libft_Status_Features.xlsx
+++ b/libft/doc/Libft_Status_Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pmicloud-my.sharepoint.com/personal/ybensegh_pmintl_net/Documents/Documents/Perso/ybensegh42/libft/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_FA7B0602B1E3D414C38F2ECD8BB25673469C3A16" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D910071-0F04-453F-A6F9-D4A32A2BE283}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_FA7B0602B1E3D414C38F2ECD8BB25673469C3A16" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E0461BA-DE79-472A-B425-593938D28253}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,16 +191,16 @@
     <t>ft_itoa</t>
   </si>
   <si>
+    <t>ft_strmapi</t>
+  </si>
+  <si>
+    <t>ft_putchar_fd</t>
+  </si>
+  <si>
     <t>Not Done</t>
   </si>
   <si>
     <t>Not Valid</t>
-  </si>
-  <si>
-    <t>ft_strmapi</t>
-  </si>
-  <si>
-    <t>ft_putchar_fd</t>
   </si>
   <si>
     <t>ft_putstr_fd</t>
@@ -746,7 +746,7 @@
   <dimension ref="B2:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
@@ -1458,7 +1458,7 @@
         <v>14</v>
       </c>
       <c r="H48" s="3">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="I48" s="3"/>
     </row>
@@ -1470,16 +1470,16 @@
         <v>50</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H49" s="3">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="I49" s="3"/>
     </row>
@@ -1488,19 +1488,19 @@
         <v>1</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H50" s="3">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="I50" s="3"/>
     </row>
@@ -1509,13 +1509,13 @@
         <v>1</v>
       </c>
       <c r="D51" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>14</v>
@@ -1533,10 +1533,10 @@
         <v>55</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>14</v>
@@ -1554,10 +1554,10 @@
         <v>56</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>23</v>
@@ -1575,10 +1575,10 @@
         <v>57</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>23</v>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="H55">
         <f>SUM(H45:H54)</f>
-        <v>2.25</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="57" spans="2:9">
@@ -1606,7 +1606,7 @@
     <row r="58" spans="2:9">
       <c r="I58" s="4">
         <f>H55/B55</f>
-        <v>0.20454545454545456</v>
+        <v>0.40909090909090912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add last functions to match mandatory part 1 and 2
</commit_message>
<xml_diff>
--- a/libft/doc/Libft_Status_Features.xlsx
+++ b/libft/doc/Libft_Status_Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pmicloud-my.sharepoint.com/personal/ybensegh_pmintl_net/Documents/Documents/Perso/ybensegh42/libft/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_FA7B0602B1E3D414C38F2ECD8BB25673469C3A16" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E0461BA-DE79-472A-B425-593938D28253}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_FA7B0602B1E3D414C38F2ECD8BB25673469C3A16" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D25ED752-4CDB-4E10-A5F5-83C765025C4A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14805" yWindow="-16425" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="56">
   <si>
     <t>Author</t>
   </si>
@@ -195,12 +195,6 @@
   </si>
   <si>
     <t>ft_putchar_fd</t>
-  </si>
-  <si>
-    <t>Not Done</t>
-  </si>
-  <si>
-    <t>Not Valid</t>
   </si>
   <si>
     <t>ft_putstr_fd</t>
@@ -219,7 +213,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -745,23 +739,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G62" sqref="G61:G62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" customWidth="1"/>
     <col min="9" max="9" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -769,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>2</v>
       </c>
@@ -777,12 +771,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>1</v>
       </c>
@@ -805,7 +799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>1</v>
       </c>
@@ -826,7 +820,7 @@
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>1</v>
       </c>
@@ -847,7 +841,7 @@
       </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>1</v>
       </c>
@@ -868,7 +862,7 @@
       </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>1</v>
       </c>
@@ -889,7 +883,7 @@
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>1</v>
       </c>
@@ -910,7 +904,7 @@
       </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>1</v>
       </c>
@@ -931,7 +925,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>1</v>
       </c>
@@ -952,7 +946,7 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>1</v>
       </c>
@@ -973,7 +967,7 @@
       </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>1</v>
       </c>
@@ -994,7 +988,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="2:9">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>1</v>
       </c>
@@ -1015,7 +1009,7 @@
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>1</v>
       </c>
@@ -1036,7 +1030,7 @@
       </c>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>1</v>
       </c>
@@ -1057,7 +1051,7 @@
       </c>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>1</v>
       </c>
@@ -1078,7 +1072,7 @@
       </c>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>1</v>
       </c>
@@ -1099,7 +1093,7 @@
       </c>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>1</v>
       </c>
@@ -1120,7 +1114,7 @@
       </c>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>1</v>
       </c>
@@ -1141,7 +1135,7 @@
       </c>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>1</v>
       </c>
@@ -1162,7 +1156,7 @@
       </c>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="2:9">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>1</v>
       </c>
@@ -1183,7 +1177,7 @@
       </c>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>1</v>
       </c>
@@ -1206,7 +1200,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="2:9">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>1</v>
       </c>
@@ -1229,7 +1223,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28">
         <v>1</v>
       </c>
@@ -1252,7 +1246,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>1</v>
       </c>
@@ -1273,7 +1267,7 @@
       </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="2:9" hidden="1">
+    <row r="30" spans="2:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="B30">
         <f>SUM(B7:B29)</f>
         <v>23</v>
@@ -1283,18 +1277,18 @@
         <v>15.75</v>
       </c>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I33" s="4">
         <f>H30/B30</f>
         <v>0.68478260869565222</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="D35" s="1" t="s">
         <v>5</v>
       </c>
@@ -1314,7 +1308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="D36" s="3" t="s">
         <v>43</v>
       </c>
@@ -1332,7 +1326,7 @@
       </c>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="D37" s="3" t="s">
         <v>44</v>
       </c>
@@ -1350,12 +1344,12 @@
       </c>
       <c r="I37" s="3"/>
     </row>
-    <row r="42" spans="2:9">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="D42" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="2:9">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B44">
         <v>1</v>
       </c>
@@ -1378,7 +1372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="2:9">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B45">
         <v>1</v>
       </c>
@@ -1399,7 +1393,7 @@
       </c>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="2:9">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B46">
         <v>1</v>
       </c>
@@ -1420,7 +1414,7 @@
       </c>
       <c r="I46" s="3"/>
     </row>
-    <row r="47" spans="2:9">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B47">
         <v>1</v>
       </c>
@@ -1441,7 +1435,7 @@
       </c>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="2:9">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B48">
         <v>1</v>
       </c>
@@ -1462,7 +1456,7 @@
       </c>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="2:9">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49">
         <v>1</v>
       </c>
@@ -1483,7 +1477,7 @@
       </c>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="2:9">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B50">
         <v>1</v>
       </c>
@@ -1504,7 +1498,7 @@
       </c>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="2:9">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B51">
         <v>1</v>
       </c>
@@ -1512,10 +1506,10 @@
         <v>52</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>14</v>
@@ -1525,18 +1519,18 @@
       </c>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="2:9">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52">
         <v>1</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>14</v>
@@ -1546,18 +1540,18 @@
       </c>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="2:9">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53">
         <v>1</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>23</v>
@@ -1567,18 +1561,18 @@
       </c>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="2:9">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54">
         <v>1</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>23</v>
@@ -1588,7 +1582,7 @@
       </c>
       <c r="I54" s="3"/>
     </row>
-    <row r="55" spans="2:9">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B55">
         <f>SUM(B44:B54)</f>
         <v>11</v>
@@ -1598,12 +1592,12 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="57" spans="2:9">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I57" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="58" spans="2:9">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I58" s="4">
         <f>H55/B55</f>
         <v>0.40909090909090912</v>

</xml_diff>